<commit_message>
Edit Energy Audit report
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy-new\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFAD5E9-0978-479F-B396-EDC460F83D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D2C21-2A99-41B6-A9AD-9DD6ACEFEABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>path to image</t>
   </si>
@@ -33,21 +33,6 @@
     <t>Path to image comment</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Adress/Name</t>
-  </si>
-  <si>
-    <t>Auditor full name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date </t>
-  </si>
-  <si>
-    <t>Combustion Gas Spillage Test</t>
-  </si>
-  <si>
     <t>Seconds of Combustion Gas Spillage Test</t>
   </si>
   <si>
@@ -76,6 +61,126 @@
   </si>
   <si>
     <t>Cooling load</t>
+  </si>
+  <si>
+    <t>Building Photo</t>
+  </si>
+  <si>
+    <t>path to photo</t>
+  </si>
+  <si>
+    <t>Window type</t>
+  </si>
+  <si>
+    <t>Window area</t>
+  </si>
+  <si>
+    <t>Door type</t>
+  </si>
+  <si>
+    <t>Door area</t>
+  </si>
+  <si>
+    <t>Net wall area</t>
+  </si>
+  <si>
+    <t>Ceiling/attic area</t>
+  </si>
+  <si>
+    <t>Basement area</t>
+  </si>
+  <si>
+    <t>Basment type</t>
+  </si>
+  <si>
+    <t>Combustion Appliance Draft Test (PASSED/FAILED)</t>
+  </si>
+  <si>
+    <t>Attics/Ceilings R-value</t>
+  </si>
+  <si>
+    <t>Above Ground Walls R-value</t>
+  </si>
+  <si>
+    <t>Basement Walls R-value</t>
+  </si>
+  <si>
+    <t>Basement Ceilings R-value</t>
+  </si>
+  <si>
+    <t>CFM50 reading</t>
+  </si>
+  <si>
+    <t>Ring Used</t>
+  </si>
+  <si>
+    <t>Image of Ring</t>
+  </si>
+  <si>
+    <t>Gas leak detection(PASSED/FAILED)</t>
+  </si>
+  <si>
+    <t>Me_test1</t>
+  </si>
+  <si>
+    <t>ME_test2</t>
+  </si>
+  <si>
+    <t>Adress_Name</t>
+  </si>
+  <si>
+    <t>Image_1</t>
+  </si>
+  <si>
+    <t>Image_2</t>
+  </si>
+  <si>
+    <t>Rudolfs</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>no_idea</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Crawlspace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audit_Date </t>
+  </si>
+  <si>
+    <t>Yearly_Energy_Cost</t>
+  </si>
+  <si>
+    <t>Year_Build</t>
+  </si>
+  <si>
+    <t>Total_floor_area</t>
+  </si>
+  <si>
+    <t>Heating_Type</t>
+  </si>
+  <si>
+    <t>Ceiling_height</t>
+  </si>
+  <si>
+    <t>Auditor_full_name</t>
   </si>
 </sst>
 </file>
@@ -111,9 +216,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -396,85 +504,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" zoomScale="40" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="15" width="9.23046875" style="1"/>
+    <col min="16" max="16" width="10.53515625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="78.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:38" ht="78.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="T1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="X1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="30.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>16</v>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45437</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="1">
+        <v>200</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1">
+        <v>300</v>
+      </c>
+      <c r="N2" s="1">
+        <v>600</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>750</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="30.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45436</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1">
+        <v>400</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="1">
+        <v>500</v>
+      </c>
+      <c r="N3" s="1">
+        <v>500</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{3E27FD5B-719B-4B8A-9435-F197BD246063}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L128:L1048576" xr:uid="{3E27FD5B-719B-4B8A-9435-F197BD246063}">
       <formula1>"PASSED, FAILED"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{71D67195-879C-49C1-8FEC-AD86EBEFACA0}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M128:M1048576" xr:uid="{71D67195-879C-49C1-8FEC-AD86EBEFACA0}">
       <formula1>1</formula1>
       <formula2>999999999999999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:Q1048576" xr:uid="{5D5DBC07-ACAF-4A74-A9D2-D6E0388A55DC}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q128:Q1048576" xr:uid="{5D5DBC07-ACAF-4A74-A9D2-D6E0388A55DC}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Work on rendering setup
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy-new\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D2C21-2A99-41B6-A9AD-9DD6ACEFEABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837E297-6528-40E6-BFD0-E4C939553AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,30 +69,6 @@
     <t>path to photo</t>
   </si>
   <si>
-    <t>Window type</t>
-  </si>
-  <si>
-    <t>Window area</t>
-  </si>
-  <si>
-    <t>Door type</t>
-  </si>
-  <si>
-    <t>Door area</t>
-  </si>
-  <si>
-    <t>Net wall area</t>
-  </si>
-  <si>
-    <t>Ceiling/attic area</t>
-  </si>
-  <si>
-    <t>Basement area</t>
-  </si>
-  <si>
-    <t>Basment type</t>
-  </si>
-  <si>
     <t>Combustion Appliance Draft Test (PASSED/FAILED)</t>
   </si>
   <si>
@@ -181,6 +157,30 @@
   </si>
   <si>
     <t>Auditor_full_name</t>
+  </si>
+  <si>
+    <t>Window_type</t>
+  </si>
+  <si>
+    <t>Window_area</t>
+  </si>
+  <si>
+    <t>Door_type</t>
+  </si>
+  <si>
+    <t>Door_area</t>
+  </si>
+  <si>
+    <t>Net_wall_area</t>
+  </si>
+  <si>
+    <t>Ceiling/attic_area</t>
+  </si>
+  <si>
+    <t>Basment_type</t>
+  </si>
+  <si>
+    <t>Basement_area</t>
   </si>
 </sst>
 </file>
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -522,52 +522,52 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>
@@ -579,10 +579,10 @@
         <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>5</v>
@@ -591,13 +591,13 @@
         <v>6</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>7</v>
@@ -615,22 +615,22 @@
         <v>11</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="AL1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="30.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -638,10 +638,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2">
         <v>45437</v>
@@ -656,19 +656,19 @@
         <v>3000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="K2" s="1">
         <v>200</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M2" s="1">
         <v>300</v>
@@ -680,7 +680,7 @@
         <v>1000</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="1">
         <v>750</v>
@@ -697,10 +697,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <v>45436</v>
@@ -715,19 +715,19 @@
         <v>5000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="M3" s="1">
         <v>500</v>
@@ -739,7 +739,7 @@
         <v>2000</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Energy report render file
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy-new\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3837E297-6528-40E6-BFD0-E4C939553AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F3169-9277-453A-81D2-675055773A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>Me_test1</t>
   </si>
   <si>
-    <t>ME_test2</t>
-  </si>
-  <si>
     <t>Adress_Name</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Basement_area</t>
+  </si>
+  <si>
+    <t>Me_test2</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -522,52 +522,52 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>
@@ -627,10 +627,10 @@
         <v>18</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="30.45" customHeight="1" x14ac:dyDescent="0.4">
@@ -641,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2">
         <v>45437</v>
@@ -656,19 +656,19 @@
         <v>3000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1">
         <v>200</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1">
         <v>300</v>
@@ -680,7 +680,7 @@
         <v>1000</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="1">
         <v>750</v>
@@ -697,10 +697,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <v>45436</v>
@@ -715,19 +715,19 @@
         <v>5000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M3" s="1">
         <v>500</v>
@@ -739,7 +739,7 @@
         <v>2000</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit params in Energy Report
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy-new\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C228DF85-3FD5-45D5-8219-F923AA8FBB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2CB5DB-8CC0-4383-97F1-DC53EC22A236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>path to image</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Me_test2</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -507,7 +516,7 @@
   <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -685,9 +694,60 @@
       <c r="Q2" s="1">
         <v>750</v>
       </c>
+      <c r="R2" s="1">
+        <v>60</v>
+      </c>
+      <c r="T2" s="1">
+        <v>20</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="1">
+        <v>600</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>500</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>400</v>
+      </c>
       <c r="AA2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AB2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>30</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>20</v>
+      </c>
       <c r="AK2" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +755,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:38" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
@@ -740,6 +803,69 @@
       </c>
       <c r="P3" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>600</v>
+      </c>
+      <c r="R3" s="1">
+        <v>50</v>
+      </c>
+      <c r="T3" s="1">
+        <v>20</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="1">
+        <v>700</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>450</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>15000</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>50</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>20</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>20</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>20</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add df reference to Heating and Cooling paragraph
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2CB5DB-8CC0-4383-97F1-DC53EC22A236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130E2766-966A-4945-9D0E-15197673597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>path to image</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -515,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AL7" sqref="AL7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -715,8 +721,8 @@
       <c r="Y2" s="1">
         <v>500</v>
       </c>
-      <c r="Z2" s="1">
-        <v>400</v>
+      <c r="Z2" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>0</v>
@@ -828,8 +834,8 @@
       <c r="Y3" s="1">
         <v>450</v>
       </c>
-      <c r="Z3" s="1">
-        <v>300</v>
+      <c r="Z3" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Render the automatic reports
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587A9126-BE9F-4CEB-AFEF-059E83E77E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B6FAA-7B98-4BDC-B93F-005C09B084B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>path to image</t>
   </si>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -855,6 +855,9 @@
       <c r="V3" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="W3" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="X3" s="1" t="s">
         <v>54</v>
       </c>
@@ -902,6 +905,9 @@
       </c>
       <c r="AM3" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the first two pages of report template
</commit_message>
<xml_diff>
--- a/data/Energy_Audit_template.xlsx
+++ b/data/Energy_Audit_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\CEDS-Energy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudolfs Lukasevics\Desktop\Repos\Quarto_report\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B6FAA-7B98-4BDC-B93F-005C09B084B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17CB88E-2462-4872-A65B-839337CB5C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Gas leak detection(PASSED/FAILED)</t>
   </si>
   <si>
-    <t>Me_test1</t>
-  </si>
-  <si>
     <t>Adress_Name</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Basement_area</t>
   </si>
   <si>
-    <t>Me_test2</t>
-  </si>
-  <si>
     <t>PASSED</t>
   </si>
   <si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>In the kitchen</t>
+  </si>
+  <si>
+    <t>Me_summer_test1</t>
+  </si>
+  <si>
+    <t>Me_summer_test2</t>
   </si>
 </sst>
 </file>
@@ -533,68 +533,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="15" width="9.23046875" style="1"/>
-    <col min="16" max="16" width="10.53515625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="15" width="9.26953125" style="1"/>
+    <col min="16" max="16" width="10.54296875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="78.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:40" ht="78.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>
@@ -612,7 +612,7 @@
         <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>5</v>
@@ -657,24 +657,24 @@
         <v>18</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="AN1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="30.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:40" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>45437</v>
@@ -689,19 +689,19 @@
         <v>3000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1">
         <v>200</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="1">
         <v>300</v>
@@ -713,7 +713,7 @@
         <v>1000</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1">
         <v>750</v>
@@ -728,16 +728,16 @@
         <v>20</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="Y2" s="1">
         <v>0.5</v>
@@ -746,13 +746,13 @@
         <v>500</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD2" s="1">
         <v>50</v>
@@ -785,18 +785,18 @@
         <v>1</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:40" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2">
         <v>45436</v>
@@ -811,19 +811,19 @@
         <v>5000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" s="1">
         <v>500</v>
@@ -835,7 +835,7 @@
         <v>2000</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="1">
         <v>600</v>
@@ -850,16 +850,16 @@
         <v>20</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="X3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y3" s="1">
         <v>0.7</v>
@@ -868,13 +868,13 @@
         <v>450</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AD3" s="1">
         <v>20</v>
@@ -907,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>